<commit_message>
Leaflet map has added for extremist permanent address
</commit_message>
<xml_diff>
--- a/data/Network_Database.xlsx
+++ b/data/Network_Database.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034ED442-086D-4555-8665-BADF2C8A47B9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CB506B-2A4F-4ECE-97A2-C365FA31B9EB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extremist_Profile" sheetId="1" r:id="rId1"/>
@@ -1640,9 +1640,6 @@
     <t>NID/Passport/Tenant Form/Other ID Faked?</t>
   </si>
   <si>
-    <t>Permanent Address</t>
-  </si>
-  <si>
     <t>Educational Institutes</t>
   </si>
   <si>
@@ -2429,6 +2426,9 @@
   </si>
   <si>
     <t>Computer Trader</t>
+  </si>
+  <si>
+    <t>PermanentAddress</t>
   </si>
 </sst>
 </file>
@@ -2969,9 +2969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN26"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P1" sqref="P1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3052,43 +3052,43 @@
         <v>397</v>
       </c>
       <c r="O1" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="P1" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>399</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>400</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>401</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="T1" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="U1" s="14" t="s">
         <v>403</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>404</v>
       </c>
       <c r="V1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="W1" s="40" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="Y1" s="14" t="s">
+        <v>405</v>
+      </c>
+      <c r="Z1" s="14" t="s">
         <v>406</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AA1" s="14" t="s">
         <v>407</v>
-      </c>
-      <c r="AA1" s="14" t="s">
-        <v>408</v>
       </c>
       <c r="AB1" s="14" t="s">
         <v>3</v>
@@ -3103,49 +3103,49 @@
         <v>6</v>
       </c>
       <c r="AF1" s="14" t="s">
+        <v>408</v>
+      </c>
+      <c r="AG1" s="14" t="s">
         <v>409</v>
       </c>
-      <c r="AG1" s="14" t="s">
+      <c r="AH1" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AI1" s="14" t="s">
         <v>411</v>
       </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="AJ1" s="14" t="s">
+      <c r="AK1" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="AK1" s="14" t="s">
+      <c r="AL1" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="AL1" s="14" t="s">
+      <c r="AM1" s="14" t="s">
         <v>415</v>
       </c>
-      <c r="AM1" s="14" t="s">
+      <c r="AN1" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="AN1" s="14" t="s">
+      <c r="AO1" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="AO1" s="14" t="s">
+      <c r="AP1" s="14" t="s">
         <v>418</v>
       </c>
-      <c r="AP1" s="14" t="s">
+      <c r="AQ1" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="AQ1" s="14" t="s">
+      <c r="AR1" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="AR1" s="14" t="s">
+      <c r="AS1" s="14" t="s">
         <v>421</v>
       </c>
-      <c r="AS1" s="14" t="s">
+      <c r="AT1" s="14" t="s">
         <v>422</v>
-      </c>
-      <c r="AT1" s="14" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:46" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3183,7 +3183,7 @@
         <v>13</v>
       </c>
       <c r="L2" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M2" s="36" t="s">
         <v>9</v>
@@ -3192,10 +3192,10 @@
         <v>9</v>
       </c>
       <c r="O2" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P2" s="46" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="Q2" s="15" t="s">
         <v>15</v>
@@ -3210,7 +3210,7 @@
         <v>18</v>
       </c>
       <c r="U2" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="V2" s="15" t="s">
         <v>19</v>
@@ -3222,7 +3222,7 @@
         <v>20</v>
       </c>
       <c r="Y2" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="Z2" s="15" t="s">
         <v>21</v>
@@ -3243,7 +3243,7 @@
         <v>25</v>
       </c>
       <c r="AF2" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG2" s="15" t="s">
         <v>26</v>
@@ -3273,19 +3273,19 @@
         <v>261</v>
       </c>
       <c r="AP2" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ2" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR2" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS2" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT2" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="3" spans="1:46" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -3323,7 +3323,7 @@
         <v>13</v>
       </c>
       <c r="L3" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M3" s="36" t="s">
         <v>9</v>
@@ -3332,10 +3332,10 @@
         <v>9</v>
       </c>
       <c r="O3" s="15" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="P3" s="46" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="Q3" s="15" t="s">
         <v>37</v>
@@ -3350,7 +3350,7 @@
         <v>39</v>
       </c>
       <c r="U3" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="V3" s="15" t="s">
         <v>19</v>
@@ -3368,7 +3368,7 @@
         <v>41</v>
       </c>
       <c r="AA3" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AB3" s="15" t="s">
         <v>42</v>
@@ -3383,7 +3383,7 @@
         <v>25</v>
       </c>
       <c r="AF3" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG3" s="15" t="s">
         <v>44</v>
@@ -3416,16 +3416,16 @@
         <v>51</v>
       </c>
       <c r="AQ3" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR3" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS3" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT3" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="4" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3463,7 +3463,7 @@
         <v>13</v>
       </c>
       <c r="L4" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M4" s="36" t="s">
         <v>9</v>
@@ -3472,7 +3472,7 @@
         <v>9</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="P4" s="15" t="s">
         <v>53</v>
@@ -3490,7 +3490,7 @@
         <v>18</v>
       </c>
       <c r="U4" s="15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="V4" s="15" t="s">
         <v>19</v>
@@ -3502,7 +3502,7 @@
         <v>20</v>
       </c>
       <c r="Y4" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="Z4" s="15" t="s">
         <v>55</v>
@@ -3523,7 +3523,7 @@
         <v>25</v>
       </c>
       <c r="AF4" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG4" s="15" t="s">
         <v>44</v>
@@ -3553,19 +3553,19 @@
         <v>261</v>
       </c>
       <c r="AP4" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ4" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR4" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS4" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT4" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="5" spans="1:46" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3603,7 +3603,7 @@
         <v>13</v>
       </c>
       <c r="L5" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M5" s="36" t="s">
         <v>9</v>
@@ -3615,7 +3615,7 @@
         <v>64</v>
       </c>
       <c r="P5" s="46" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q5" s="15" t="s">
         <v>15</v>
@@ -3630,7 +3630,7 @@
         <v>66</v>
       </c>
       <c r="U5" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="V5" s="15" t="s">
         <v>19</v>
@@ -3648,7 +3648,7 @@
         <v>68</v>
       </c>
       <c r="AA5" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AB5" s="15" t="s">
         <v>69</v>
@@ -3663,7 +3663,7 @@
         <v>25</v>
       </c>
       <c r="AF5" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG5" s="15" t="s">
         <v>44</v>
@@ -3687,25 +3687,25 @@
         <v>13</v>
       </c>
       <c r="AN5" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AO5" s="15" t="s">
         <v>73</v>
       </c>
       <c r="AP5" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ5" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR5" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS5" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT5" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="6" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3743,7 +3743,7 @@
         <v>13</v>
       </c>
       <c r="L6" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M6" s="36" t="s">
         <v>9</v>
@@ -3752,7 +3752,7 @@
         <v>9</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="P6" s="15" t="s">
         <v>75</v>
@@ -3770,7 +3770,7 @@
         <v>66</v>
       </c>
       <c r="U6" s="15" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="V6" s="15" t="s">
         <v>19</v>
@@ -3803,7 +3803,7 @@
         <v>25</v>
       </c>
       <c r="AF6" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG6" s="15" t="s">
         <v>78</v>
@@ -3827,25 +3827,25 @@
         <v>13</v>
       </c>
       <c r="AN6" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AO6" s="15" t="s">
         <v>81</v>
       </c>
       <c r="AP6" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ6" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR6" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS6" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT6" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="7" spans="1:46" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -3883,7 +3883,7 @@
         <v>13</v>
       </c>
       <c r="L7" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M7" s="36" t="s">
         <v>9</v>
@@ -3895,10 +3895,10 @@
         <v>85</v>
       </c>
       <c r="P7" s="46" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="R7" s="15" t="s">
         <v>16</v>
@@ -3910,7 +3910,7 @@
         <v>87</v>
       </c>
       <c r="U7" s="15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="V7" s="15" t="s">
         <v>19</v>
@@ -3922,13 +3922,13 @@
         <v>88</v>
       </c>
       <c r="Y7" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="Z7" s="15" t="s">
         <v>89</v>
       </c>
       <c r="AA7" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AB7" s="15" t="s">
         <v>77</v>
@@ -3943,7 +3943,7 @@
         <v>25</v>
       </c>
       <c r="AF7" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG7" s="15" t="s">
         <v>44</v>
@@ -3976,16 +3976,16 @@
         <v>94</v>
       </c>
       <c r="AQ7" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR7" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS7" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT7" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="8" spans="1:46" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4023,7 +4023,7 @@
         <v>13</v>
       </c>
       <c r="L8" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M8" s="36" t="s">
         <v>9</v>
@@ -4032,10 +4032,10 @@
         <v>9</v>
       </c>
       <c r="O8" s="15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="P8" s="46" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="Q8" s="15" t="s">
         <v>98</v>
@@ -4050,7 +4050,7 @@
         <v>100</v>
       </c>
       <c r="U8" s="15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="V8" s="15" t="s">
         <v>19</v>
@@ -4062,7 +4062,7 @@
         <v>20</v>
       </c>
       <c r="Y8" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="Z8" s="15" t="s">
         <v>101</v>
@@ -4083,7 +4083,7 @@
         <v>25</v>
       </c>
       <c r="AF8" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG8" s="15" t="s">
         <v>102</v>
@@ -4113,19 +4113,19 @@
         <v>50</v>
       </c>
       <c r="AP8" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ8" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR8" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS8" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT8" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="9" spans="1:46" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4157,13 +4157,13 @@
         <v>13</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K9" s="36" t="s">
         <v>13</v>
       </c>
       <c r="L9" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M9" s="36" t="s">
         <v>9</v>
@@ -4175,10 +4175,10 @@
         <v>111</v>
       </c>
       <c r="P9" s="15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="R9" s="15" t="s">
         <v>112</v>
@@ -4190,7 +4190,7 @@
         <v>114</v>
       </c>
       <c r="U9" s="15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="V9" s="15" t="s">
         <v>19</v>
@@ -4223,7 +4223,7 @@
         <v>25</v>
       </c>
       <c r="AF9" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG9" s="15" t="s">
         <v>119</v>
@@ -4235,7 +4235,7 @@
         <v>120</v>
       </c>
       <c r="AJ9" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AK9" s="15" t="s">
         <v>121</v>
@@ -4256,16 +4256,16 @@
         <v>94</v>
       </c>
       <c r="AQ9" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR9" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS9" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT9" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="10" spans="1:46" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -4303,7 +4303,7 @@
         <v>13</v>
       </c>
       <c r="L10" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M10" s="36" t="s">
         <v>9</v>
@@ -4315,10 +4315,10 @@
         <v>125</v>
       </c>
       <c r="P10" s="46" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="R10" s="15" t="s">
         <v>112</v>
@@ -4330,7 +4330,7 @@
         <v>127</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="V10" s="15" t="s">
         <v>19</v>
@@ -4342,10 +4342,10 @@
         <v>20</v>
       </c>
       <c r="Y10" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="Z10" s="15" t="s">
         <v>563</v>
-      </c>
-      <c r="Z10" s="15" t="s">
-        <v>564</v>
       </c>
       <c r="AA10" s="15" t="s">
         <v>133</v>
@@ -4363,7 +4363,7 @@
         <v>25</v>
       </c>
       <c r="AF10" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG10" s="15" t="s">
         <v>129</v>
@@ -4375,7 +4375,7 @@
         <v>45</v>
       </c>
       <c r="AJ10" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AK10" s="15" t="s">
         <v>104</v>
@@ -4396,16 +4396,16 @@
         <v>132</v>
       </c>
       <c r="AQ10" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR10" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS10" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT10" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11" spans="1:46" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4443,7 +4443,7 @@
         <v>13</v>
       </c>
       <c r="L11" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M11" s="36" t="s">
         <v>9</v>
@@ -4452,13 +4452,13 @@
         <v>9</v>
       </c>
       <c r="O11" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="P11" s="46" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="Q11" s="15" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="R11" s="15" t="s">
         <v>16</v>
@@ -4470,7 +4470,7 @@
         <v>114</v>
       </c>
       <c r="U11" s="15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V11" s="15" t="s">
         <v>19</v>
@@ -4482,7 +4482,7 @@
         <v>20</v>
       </c>
       <c r="Y11" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="Z11" s="15" t="s">
         <v>139</v>
@@ -4503,7 +4503,7 @@
         <v>25</v>
       </c>
       <c r="AF11" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG11" s="15" t="s">
         <v>44</v>
@@ -4533,19 +4533,19 @@
         <v>261</v>
       </c>
       <c r="AP11" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ11" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR11" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS11" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT11" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="12" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4583,7 +4583,7 @@
         <v>13</v>
       </c>
       <c r="L12" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M12" s="36" t="s">
         <v>9</v>
@@ -4598,7 +4598,7 @@
         <v>149</v>
       </c>
       <c r="Q12" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="R12" s="15" t="s">
         <v>16</v>
@@ -4610,7 +4610,7 @@
         <v>151</v>
       </c>
       <c r="U12" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="V12" s="15" t="s">
         <v>19</v>
@@ -4622,7 +4622,7 @@
         <v>20</v>
       </c>
       <c r="Y12" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="Z12" s="15" t="s">
         <v>152</v>
@@ -4643,7 +4643,7 @@
         <v>25</v>
       </c>
       <c r="AF12" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG12" s="15" t="s">
         <v>44</v>
@@ -4667,25 +4667,25 @@
         <v>260</v>
       </c>
       <c r="AN12" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AO12" s="15" t="s">
         <v>155</v>
       </c>
       <c r="AP12" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ12" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR12" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS12" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT12" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="13" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4723,7 +4723,7 @@
         <v>13</v>
       </c>
       <c r="L13" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M13" s="36" t="s">
         <v>9</v>
@@ -4732,7 +4732,7 @@
         <v>9</v>
       </c>
       <c r="O13" s="15" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="P13" s="15" t="s">
         <v>161</v>
@@ -4750,7 +4750,7 @@
         <v>164</v>
       </c>
       <c r="U13" s="15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="V13" s="15" t="s">
         <v>19</v>
@@ -4759,7 +4759,7 @@
         <v>22</v>
       </c>
       <c r="X13" s="15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Y13" s="5" t="s">
         <v>68</v>
@@ -4783,7 +4783,7 @@
         <v>25</v>
       </c>
       <c r="AF13" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG13" s="15" t="s">
         <v>44</v>
@@ -4795,7 +4795,7 @@
         <v>45</v>
       </c>
       <c r="AJ13" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AK13" s="15" t="s">
         <v>72</v>
@@ -4816,16 +4816,16 @@
         <v>169</v>
       </c>
       <c r="AQ13" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR13" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS13" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT13" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="14" spans="1:46" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -4863,7 +4863,7 @@
         <v>13</v>
       </c>
       <c r="L14" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M14" s="36" t="s">
         <v>9</v>
@@ -4875,7 +4875,7 @@
         <v>172</v>
       </c>
       <c r="P14" s="46" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="Q14" s="15" t="s">
         <v>173</v>
@@ -4902,13 +4902,13 @@
         <v>20</v>
       </c>
       <c r="Y14" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="Z14" s="15" t="s">
         <v>176</v>
       </c>
       <c r="AA14" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AB14" s="15" t="s">
         <v>22</v>
@@ -4923,7 +4923,7 @@
         <v>25</v>
       </c>
       <c r="AF14" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG14" s="15" t="s">
         <v>44</v>
@@ -4947,25 +4947,25 @@
         <v>180</v>
       </c>
       <c r="AN14" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AO14" s="15" t="s">
         <v>261</v>
       </c>
       <c r="AP14" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ14" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR14" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS14" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT14" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="15" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5003,7 +5003,7 @@
         <v>13</v>
       </c>
       <c r="L15" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M15" s="36" t="s">
         <v>9</v>
@@ -5012,10 +5012,10 @@
         <v>9</v>
       </c>
       <c r="O15" s="15" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="P15" s="15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Q15" s="15" t="s">
         <v>185</v>
@@ -5030,7 +5030,7 @@
         <v>114</v>
       </c>
       <c r="U15" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="V15" s="15" t="s">
         <v>19</v>
@@ -5045,10 +5045,10 @@
         <v>188</v>
       </c>
       <c r="Z15" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AA15" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AB15" s="15" t="s">
         <v>77</v>
@@ -5063,7 +5063,7 @@
         <v>25</v>
       </c>
       <c r="AF15" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG15" s="15" t="s">
         <v>44</v>
@@ -5075,7 +5075,7 @@
         <v>45</v>
       </c>
       <c r="AJ15" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AK15" s="15" t="s">
         <v>72</v>
@@ -5096,16 +5096,16 @@
         <v>94</v>
       </c>
       <c r="AQ15" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR15" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS15" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT15" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="16" spans="1:46" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -5143,7 +5143,7 @@
         <v>13</v>
       </c>
       <c r="L16" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M16" s="36" t="s">
         <v>9</v>
@@ -5152,10 +5152,10 @@
         <v>9</v>
       </c>
       <c r="O16" s="15" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="P16" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q16" s="15" t="s">
         <v>196</v>
@@ -5170,7 +5170,7 @@
         <v>198</v>
       </c>
       <c r="U16" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="V16" s="15" t="s">
         <v>19</v>
@@ -5203,7 +5203,7 @@
         <v>25</v>
       </c>
       <c r="AF16" s="16" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AG16" s="15" t="s">
         <v>44</v>
@@ -5215,7 +5215,7 @@
         <v>201</v>
       </c>
       <c r="AJ16" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AK16" s="15" t="s">
         <v>46</v>
@@ -5233,19 +5233,19 @@
         <v>275</v>
       </c>
       <c r="AP16" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ16" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR16" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS16" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT16" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="17" spans="1:66" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -5283,7 +5283,7 @@
         <v>13</v>
       </c>
       <c r="L17" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M17" s="36" t="s">
         <v>9</v>
@@ -5295,7 +5295,7 @@
         <v>204</v>
       </c>
       <c r="P17" s="46" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="Q17" s="15" t="s">
         <v>15</v>
@@ -5310,7 +5310,7 @@
         <v>205</v>
       </c>
       <c r="U17" s="15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="V17" s="15" t="s">
         <v>19</v>
@@ -5343,7 +5343,7 @@
         <v>25</v>
       </c>
       <c r="AF17" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG17" s="15" t="s">
         <v>44</v>
@@ -5373,19 +5373,19 @@
         <v>261</v>
       </c>
       <c r="AP17" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ17" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR17" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS17" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT17" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="18" spans="1:66" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5423,7 +5423,7 @@
         <v>13</v>
       </c>
       <c r="L18" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M18" s="36" t="s">
         <v>9</v>
@@ -5432,13 +5432,13 @@
         <v>9</v>
       </c>
       <c r="O18" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="P18" s="46" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="Q18" s="15" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="R18" s="15" t="s">
         <v>112</v>
@@ -5450,7 +5450,7 @@
         <v>214</v>
       </c>
       <c r="U18" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="V18" s="15" t="s">
         <v>19</v>
@@ -5459,7 +5459,7 @@
         <v>38</v>
       </c>
       <c r="X18" s="15" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Y18" s="15" t="s">
         <v>215</v>
@@ -5468,7 +5468,7 @@
         <v>216</v>
       </c>
       <c r="AA18" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AB18" s="15" t="s">
         <v>22</v>
@@ -5483,7 +5483,7 @@
         <v>25</v>
       </c>
       <c r="AF18" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG18" s="15" t="s">
         <v>217</v>
@@ -5507,25 +5507,25 @@
         <v>222</v>
       </c>
       <c r="AN18" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AO18" s="15" t="s">
         <v>223</v>
       </c>
       <c r="AP18" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ18" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR18" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS18" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT18" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="19" spans="1:66" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5572,13 +5572,13 @@
         <v>9</v>
       </c>
       <c r="O19" s="20" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="P19" s="47" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="Q19" s="20" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="R19" s="20" t="s">
         <v>16</v>
@@ -5608,7 +5608,7 @@
         <v>21</v>
       </c>
       <c r="AA19" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AB19" s="20" t="s">
         <v>297</v>
@@ -5623,7 +5623,7 @@
         <v>25</v>
       </c>
       <c r="AF19" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG19" s="20" t="s">
         <v>298</v>
@@ -5638,7 +5638,7 @@
         <v>301</v>
       </c>
       <c r="AK19" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AL19" s="15" t="s">
         <v>260</v>
@@ -5647,25 +5647,25 @@
         <v>260</v>
       </c>
       <c r="AN19" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AO19" s="15" t="s">
         <v>260</v>
       </c>
       <c r="AP19" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ19" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR19" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS19" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT19" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="20" spans="1:66" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -5715,10 +5715,10 @@
         <v>307</v>
       </c>
       <c r="P20" s="47" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="Q20" s="20" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="R20" s="20" t="s">
         <v>308</v>
@@ -5745,7 +5745,7 @@
         <v>20</v>
       </c>
       <c r="Z20" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AA20" s="23"/>
       <c r="AB20" s="20" t="s">
@@ -5761,7 +5761,7 @@
         <v>25</v>
       </c>
       <c r="AF20" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG20" s="20" t="s">
         <v>313</v>
@@ -5773,10 +5773,10 @@
         <v>45</v>
       </c>
       <c r="AJ20" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AK20" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AL20" s="15" t="s">
         <v>260</v>
@@ -5785,25 +5785,25 @@
         <v>260</v>
       </c>
       <c r="AN20" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AO20" s="15" t="s">
         <v>260</v>
       </c>
       <c r="AP20" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ20" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AR20" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AS20" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT20" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="21" spans="1:66" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5853,10 +5853,10 @@
         <v>319</v>
       </c>
       <c r="P21" s="47" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="Q21" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="R21" s="20" t="s">
         <v>112</v>
@@ -5865,7 +5865,7 @@
         <v>320</v>
       </c>
       <c r="T21" s="20" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="U21" s="20" t="s">
         <v>321</v>
@@ -5901,7 +5901,7 @@
         <v>25</v>
       </c>
       <c r="AF21" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG21" s="20" t="s">
         <v>325</v>
@@ -5913,7 +5913,7 @@
         <v>45</v>
       </c>
       <c r="AJ21" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AK21" s="20" t="s">
         <v>326</v>
@@ -5931,7 +5931,7 @@
         <v>330</v>
       </c>
       <c r="AP21" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ21" s="20" t="s">
         <v>331</v>
@@ -5940,7 +5940,7 @@
         <v>332</v>
       </c>
       <c r="AS21" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AT21" s="22" t="s">
         <v>333</v>
@@ -5972,7 +5972,7 @@
         <v>335</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H22" s="21" t="s">
         <v>9</v>
@@ -5996,13 +5996,13 @@
         <v>13</v>
       </c>
       <c r="O22" s="20" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="P22" s="47" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="Q22" s="20" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="R22" s="20" t="s">
         <v>16</v>
@@ -6020,19 +6020,19 @@
         <v>19</v>
       </c>
       <c r="W22" s="37" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="X22" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="Y22" s="20" t="s">
         <v>338</v>
       </c>
       <c r="Z22" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AA22" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AB22" s="20" t="s">
         <v>22</v>
@@ -6047,10 +6047,10 @@
         <v>25</v>
       </c>
       <c r="AF22" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG22" s="20" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AH22" s="20" t="s">
         <v>70</v>
@@ -6059,10 +6059,10 @@
         <v>45</v>
       </c>
       <c r="AJ22" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AK22" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AL22" s="20" t="s">
         <v>339</v>
@@ -6071,13 +6071,13 @@
         <v>340</v>
       </c>
       <c r="AN22" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AO22" s="20" t="s">
         <v>341</v>
       </c>
       <c r="AP22" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ22" s="20" t="s">
         <v>342</v>
@@ -6100,7 +6100,7 @@
     </row>
     <row r="23" spans="1:66" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B23" s="37">
         <v>60</v>
@@ -6115,10 +6115,10 @@
         <v>94</v>
       </c>
       <c r="F23" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="G23" s="20" t="s">
         <v>445</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>446</v>
       </c>
       <c r="H23" s="21" t="s">
         <v>9</v>
@@ -6142,25 +6142,25 @@
         <v>13</v>
       </c>
       <c r="O23" s="20" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="P23" s="47" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="Q23" s="20" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="R23" s="20" t="s">
         <v>112</v>
       </c>
       <c r="S23" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="T23" s="20" t="s">
         <v>151</v>
       </c>
       <c r="U23" s="20" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="V23" s="20" t="s">
         <v>19</v>
@@ -6169,13 +6169,13 @@
         <v>30</v>
       </c>
       <c r="X23" s="20" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="Y23" s="20" t="s">
+        <v>449</v>
+      </c>
+      <c r="Z23" s="20" t="s">
         <v>450</v>
-      </c>
-      <c r="Z23" s="20" t="s">
-        <v>451</v>
       </c>
       <c r="AA23" s="20" t="s">
         <v>145</v>
@@ -6190,13 +6190,13 @@
         <v>24</v>
       </c>
       <c r="AE23" s="20" t="s">
+        <v>451</v>
+      </c>
+      <c r="AF23" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="AG23" s="20" t="s">
         <v>452</v>
-      </c>
-      <c r="AF23" s="20" t="s">
-        <v>563</v>
-      </c>
-      <c r="AG23" s="20" t="s">
-        <v>453</v>
       </c>
       <c r="AH23" s="20" t="s">
         <v>70</v>
@@ -6205,40 +6205,40 @@
         <v>45</v>
       </c>
       <c r="AJ23" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AK23" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AL23" s="20" t="s">
+        <v>453</v>
+      </c>
+      <c r="AM23" s="20" t="s">
         <v>454</v>
       </c>
-      <c r="AM23" s="20" t="s">
-        <v>455</v>
-      </c>
       <c r="AN23" s="22" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AO23" s="20"/>
       <c r="AP23" s="20" t="s">
+        <v>455</v>
+      </c>
+      <c r="AQ23" s="20" t="s">
         <v>456</v>
       </c>
-      <c r="AQ23" s="20" t="s">
+      <c r="AR23" s="20" t="s">
         <v>457</v>
       </c>
-      <c r="AR23" s="20" t="s">
+      <c r="AS23" s="50" t="s">
+        <v>562</v>
+      </c>
+      <c r="AT23" s="22" t="s">
         <v>458</v>
-      </c>
-      <c r="AS23" s="50" t="s">
-        <v>563</v>
-      </c>
-      <c r="AT23" s="22" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="24" spans="1:66" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="50" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B24" s="49">
         <v>35</v>
@@ -6247,16 +6247,16 @@
         <v>13</v>
       </c>
       <c r="D24" s="50" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E24" s="50" t="s">
         <v>51</v>
       </c>
       <c r="F24" s="50" t="s">
+        <v>506</v>
+      </c>
+      <c r="G24" s="50" t="s">
         <v>507</v>
-      </c>
-      <c r="G24" s="50" t="s">
-        <v>508</v>
       </c>
       <c r="H24" s="51" t="s">
         <v>9</v>
@@ -6280,25 +6280,25 @@
         <v>9</v>
       </c>
       <c r="O24" s="53" t="s">
+        <v>508</v>
+      </c>
+      <c r="P24" s="50" t="s">
         <v>509</v>
       </c>
-      <c r="P24" s="50" t="s">
+      <c r="Q24" s="50" t="s">
         <v>510</v>
-      </c>
-      <c r="Q24" s="50" t="s">
-        <v>511</v>
       </c>
       <c r="R24" s="50" t="s">
         <v>16</v>
       </c>
       <c r="S24" s="50" t="s">
+        <v>511</v>
+      </c>
+      <c r="T24" s="50" t="s">
         <v>512</v>
       </c>
-      <c r="T24" s="50" t="s">
+      <c r="U24" s="50" t="s">
         <v>513</v>
-      </c>
-      <c r="U24" s="50" t="s">
-        <v>514</v>
       </c>
       <c r="V24" s="50" t="s">
         <v>19</v>
@@ -6307,16 +6307,16 @@
         <v>30</v>
       </c>
       <c r="X24" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Y24" s="50" t="s">
         <v>20</v>
       </c>
       <c r="Z24" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AA24" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AB24" s="50" t="s">
         <v>324</v>
@@ -6331,10 +6331,10 @@
         <v>25</v>
       </c>
       <c r="AF24" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AG24" s="50" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AH24" s="50" t="s">
         <v>141</v>
@@ -6343,37 +6343,37 @@
         <v>45</v>
       </c>
       <c r="AJ24" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AK24" s="50" t="s">
         <v>46</v>
       </c>
       <c r="AL24" s="50" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AM24" s="50" t="s">
         <v>180</v>
       </c>
       <c r="AN24" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AO24" s="50" t="s">
+        <v>516</v>
+      </c>
+      <c r="AP24" s="50" t="s">
         <v>517</v>
       </c>
-      <c r="AP24" s="50" t="s">
+      <c r="AQ24" s="50" t="s">
         <v>518</v>
       </c>
-      <c r="AQ24" s="50" t="s">
+      <c r="AR24" s="50" t="s">
         <v>519</v>
       </c>
-      <c r="AR24" s="50" t="s">
+      <c r="AS24" s="50" t="s">
+        <v>562</v>
+      </c>
+      <c r="AT24" s="54" t="s">
         <v>520</v>
-      </c>
-      <c r="AS24" s="50" t="s">
-        <v>563</v>
-      </c>
-      <c r="AT24" s="54" t="s">
-        <v>521</v>
       </c>
       <c r="AU24" s="50"/>
       <c r="AV24" s="50"/>
@@ -6392,7 +6392,7 @@
     </row>
     <row r="25" spans="1:66" s="55" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B25" s="49">
         <v>24</v>
@@ -6401,16 +6401,16 @@
         <v>13</v>
       </c>
       <c r="D25" s="50" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E25" s="50" t="s">
         <v>94</v>
       </c>
       <c r="F25" s="50" t="s">
+        <v>523</v>
+      </c>
+      <c r="G25" s="50" t="s">
         <v>524</v>
-      </c>
-      <c r="G25" s="50" t="s">
-        <v>525</v>
       </c>
       <c r="H25" s="51" t="s">
         <v>13</v>
@@ -6434,28 +6434,28 @@
         <v>13</v>
       </c>
       <c r="O25" s="50" t="s">
+        <v>525</v>
+      </c>
+      <c r="P25" s="57" t="s">
+        <v>561</v>
+      </c>
+      <c r="Q25" s="50" t="s">
         <v>526</v>
-      </c>
-      <c r="P25" s="57" t="s">
-        <v>562</v>
-      </c>
-      <c r="Q25" s="50" t="s">
-        <v>527</v>
       </c>
       <c r="R25" s="50" t="s">
         <v>16</v>
       </c>
       <c r="S25" s="50" t="s">
+        <v>527</v>
+      </c>
+      <c r="T25" s="49" t="s">
+        <v>464</v>
+      </c>
+      <c r="U25" s="50" t="s">
         <v>528</v>
       </c>
-      <c r="T25" s="49" t="s">
-        <v>465</v>
-      </c>
-      <c r="U25" s="50" t="s">
+      <c r="V25" s="50" t="s">
         <v>529</v>
-      </c>
-      <c r="V25" s="50" t="s">
-        <v>530</v>
       </c>
       <c r="W25" s="51">
         <v>20</v>
@@ -6467,10 +6467,10 @@
         <v>20</v>
       </c>
       <c r="Z25" s="50" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AA25" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AB25" s="50" t="s">
         <v>324</v>
@@ -6485,49 +6485,49 @@
         <v>25</v>
       </c>
       <c r="AF25" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AG25" s="50" t="s">
+        <v>531</v>
+      </c>
+      <c r="AH25" s="50" t="s">
         <v>532</v>
       </c>
-      <c r="AH25" s="50" t="s">
+      <c r="AI25" s="50" t="s">
         <v>533</v>
       </c>
-      <c r="AI25" s="50" t="s">
+      <c r="AJ25" s="50" t="s">
+        <v>562</v>
+      </c>
+      <c r="AK25" s="54" t="s">
         <v>534</v>
       </c>
-      <c r="AJ25" s="50" t="s">
-        <v>563</v>
-      </c>
-      <c r="AK25" s="54" t="s">
+      <c r="AL25" s="50" t="s">
         <v>535</v>
       </c>
-      <c r="AL25" s="50" t="s">
+      <c r="AM25" s="50" t="s">
         <v>536</v>
       </c>
-      <c r="AM25" s="50" t="s">
-        <v>537</v>
-      </c>
       <c r="AN25" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AO25" s="50" t="s">
         <v>50</v>
       </c>
       <c r="AP25" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AQ25" s="50" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AR25" s="50" t="s">
         <v>332</v>
       </c>
       <c r="AS25" s="50" t="s">
+        <v>537</v>
+      </c>
+      <c r="AT25" s="54" t="s">
         <v>538</v>
-      </c>
-      <c r="AT25" s="54" t="s">
-        <v>539</v>
       </c>
       <c r="AU25" s="50"/>
       <c r="AV25" s="50"/>
@@ -6546,7 +6546,7 @@
     </row>
     <row r="26" spans="1:66" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B26" s="56">
         <v>31</v>
@@ -6555,16 +6555,16 @@
         <v>9</v>
       </c>
       <c r="D26" s="54" t="s">
+        <v>540</v>
+      </c>
+      <c r="E26" s="50" t="s">
         <v>541</v>
       </c>
-      <c r="E26" s="50" t="s">
+      <c r="F26" s="50" t="s">
         <v>542</v>
       </c>
-      <c r="F26" s="50" t="s">
+      <c r="G26" s="50" t="s">
         <v>543</v>
-      </c>
-      <c r="G26" s="50" t="s">
-        <v>544</v>
       </c>
       <c r="H26" s="51" t="s">
         <v>13</v>
@@ -6588,25 +6588,25 @@
         <v>13</v>
       </c>
       <c r="O26" s="50" t="s">
+        <v>544</v>
+      </c>
+      <c r="P26" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="P26" s="50" t="s">
+      <c r="Q26" s="50" t="s">
         <v>546</v>
       </c>
-      <c r="Q26" s="50" t="s">
+      <c r="R26" s="50" t="s">
         <v>547</v>
       </c>
-      <c r="R26" s="50" t="s">
+      <c r="S26" s="50" t="s">
         <v>548</v>
-      </c>
-      <c r="S26" s="50" t="s">
-        <v>549</v>
       </c>
       <c r="T26" s="50" t="s">
         <v>114</v>
       </c>
       <c r="U26" s="50" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="V26" s="50" t="s">
         <v>19</v>
@@ -6615,13 +6615,13 @@
         <v>28</v>
       </c>
       <c r="X26" s="50" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="Y26" s="50" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="Z26" s="50" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AA26" s="34" t="s">
         <v>145</v>
@@ -6639,10 +6639,10 @@
         <v>25</v>
       </c>
       <c r="AF26" s="50" t="s">
+        <v>552</v>
+      </c>
+      <c r="AG26" s="50" t="s">
         <v>553</v>
-      </c>
-      <c r="AG26" s="50" t="s">
-        <v>554</v>
       </c>
       <c r="AH26" s="50" t="s">
         <v>299</v>
@@ -6651,37 +6651,37 @@
         <v>45</v>
       </c>
       <c r="AJ26" s="50" t="s">
+        <v>554</v>
+      </c>
+      <c r="AK26" s="54" t="s">
         <v>555</v>
-      </c>
-      <c r="AK26" s="54" t="s">
-        <v>556</v>
       </c>
       <c r="AL26" s="50" t="s">
         <v>260</v>
       </c>
       <c r="AM26" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AN26" s="50" t="s">
+        <v>556</v>
+      </c>
+      <c r="AO26" s="50" t="s">
         <v>557</v>
       </c>
-      <c r="AO26" s="50" t="s">
+      <c r="AP26" s="50" t="s">
+        <v>562</v>
+      </c>
+      <c r="AQ26" s="50" t="s">
         <v>558</v>
       </c>
-      <c r="AP26" s="50" t="s">
-        <v>563</v>
-      </c>
-      <c r="AQ26" s="50" t="s">
+      <c r="AR26" s="50" t="s">
         <v>559</v>
       </c>
-      <c r="AR26" s="50" t="s">
+      <c r="AS26" s="50" t="s">
+        <v>562</v>
+      </c>
+      <c r="AT26" s="54" t="s">
         <v>560</v>
-      </c>
-      <c r="AS26" s="50" t="s">
-        <v>563</v>
-      </c>
-      <c r="AT26" s="54" t="s">
-        <v>561</v>
       </c>
       <c r="AU26" s="50"/>
       <c r="AZ26" s="50"/>
@@ -6708,8 +6708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D1AC17-E848-4874-935B-F6E7DA264F86}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6862,7 +6862,7 @@
         <v>0</v>
       </c>
       <c r="S2" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
@@ -6926,7 +6926,7 @@
       <c r="Q3" s="27"/>
       <c r="R3" s="27"/>
       <c r="S3" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T3" s="1">
         <v>0</v>
@@ -6949,7 +6949,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>231</v>
@@ -6994,7 +6994,7 @@
         <v>0</v>
       </c>
       <c r="S4" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T4" s="1">
         <v>0</v>
@@ -7017,7 +7017,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>233</v>
@@ -7060,7 +7060,7 @@
         <v>0</v>
       </c>
       <c r="S5" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T5" s="1">
         <v>0</v>
@@ -7069,7 +7069,7 @@
         <v>0</v>
       </c>
       <c r="V5" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7083,7 +7083,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>234</v>
@@ -7128,7 +7128,7 @@
         <v>0</v>
       </c>
       <c r="S6" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T6" s="1">
         <v>0</v>
@@ -7137,7 +7137,7 @@
         <v>0</v>
       </c>
       <c r="V6" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7154,7 +7154,7 @@
         <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F7" s="26">
         <v>0</v>
@@ -7196,7 +7196,7 @@
         <v>0</v>
       </c>
       <c r="S7" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T7" s="1">
         <v>0</v>
@@ -7219,7 +7219,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>235</v>
@@ -7264,7 +7264,7 @@
         <v>0</v>
       </c>
       <c r="S8" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T8" s="1">
         <v>3</v>
@@ -7331,7 +7331,7 @@
         <v>0</v>
       </c>
       <c r="S9" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T9" s="19">
         <v>2</v>
@@ -7340,7 +7340,7 @@
         <v>2</v>
       </c>
       <c r="V9" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="W9" s="19"/>
       <c r="X9" s="20"/>
@@ -7404,7 +7404,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T10" s="19">
         <v>3</v>
@@ -7578,7 +7578,7 @@
         <v>355</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>356</v>
@@ -7617,13 +7617,13 @@
         <v>6</v>
       </c>
       <c r="Q13" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="R13" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="S13" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T13" s="19">
         <v>0</v>
@@ -7718,16 +7718,16 @@
         <v>36225</v>
       </c>
       <c r="B15" s="50" t="s">
+        <v>564</v>
+      </c>
+      <c r="C15" s="50" t="s">
         <v>565</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="D15" s="50" t="s">
         <v>566</v>
       </c>
-      <c r="D15" s="50" t="s">
+      <c r="E15" s="50" t="s">
         <v>567</v>
-      </c>
-      <c r="E15" s="50" t="s">
-        <v>568</v>
       </c>
       <c r="F15" s="49">
         <v>150</v>
@@ -7748,7 +7748,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="M15" s="49">
         <v>2</v>
@@ -7760,19 +7760,19 @@
         <v>2</v>
       </c>
       <c r="P15" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="Q15" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="R15" s="49">
         <v>0</v>
       </c>
       <c r="S15" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T15" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="U15" s="49">
         <v>0</v>
@@ -7781,7 +7781,7 @@
         <v>0</v>
       </c>
       <c r="W15" s="50" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="X15" s="50"/>
       <c r="Y15" s="50"/>
@@ -7791,16 +7791,16 @@
         <v>41320</v>
       </c>
       <c r="B16" s="50" t="s">
+        <v>569</v>
+      </c>
+      <c r="C16" s="50" t="s">
         <v>570</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="D16" s="50" t="s">
+        <v>570</v>
+      </c>
+      <c r="E16" s="50" t="s">
         <v>571</v>
-      </c>
-      <c r="D16" s="50" t="s">
-        <v>571</v>
-      </c>
-      <c r="E16" s="50" t="s">
-        <v>572</v>
       </c>
       <c r="F16" s="49">
         <v>1</v>
@@ -7827,10 +7827,10 @@
         <v>1</v>
       </c>
       <c r="N16" s="50" t="s">
+        <v>572</v>
+      </c>
+      <c r="O16" s="50" t="s">
         <v>573</v>
-      </c>
-      <c r="O16" s="50" t="s">
-        <v>574</v>
       </c>
       <c r="P16" s="49">
         <v>8</v>
@@ -7842,19 +7842,19 @@
         <v>0</v>
       </c>
       <c r="S16" s="50" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="T16" s="50" t="s">
+        <v>574</v>
+      </c>
+      <c r="U16" s="49">
+        <v>0</v>
+      </c>
+      <c r="V16" s="49">
+        <v>0</v>
+      </c>
+      <c r="W16" s="50" t="s">
         <v>575</v>
-      </c>
-      <c r="U16" s="49">
-        <v>0</v>
-      </c>
-      <c r="V16" s="49">
-        <v>0</v>
-      </c>
-      <c r="W16" s="50" t="s">
-        <v>576</v>
       </c>
       <c r="X16" s="49">
         <v>8</v>
@@ -7866,16 +7866,16 @@
         <v>42061</v>
       </c>
       <c r="B17" s="50" t="s">
+        <v>576</v>
+      </c>
+      <c r="C17" s="50" t="s">
         <v>577</v>
       </c>
-      <c r="C17" s="50" t="s">
-        <v>578</v>
-      </c>
       <c r="D17" s="50" t="s">
+        <v>579</v>
+      </c>
+      <c r="E17" s="50" t="s">
         <v>580</v>
-      </c>
-      <c r="E17" s="50" t="s">
-        <v>581</v>
       </c>
       <c r="F17" s="49">
         <v>1</v>
@@ -7911,16 +7911,16 @@
         <v>4</v>
       </c>
       <c r="Q17" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="R17" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="S17" s="50" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="T17" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="U17" s="49">
         <v>0</v>
@@ -7929,7 +7929,7 @@
         <v>0</v>
       </c>
       <c r="W17" s="50" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="X17" s="49">
         <v>10</v>
@@ -8015,7 +8015,7 @@
         <v>242</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>243</v>
@@ -8041,7 +8041,7 @@
         <v>13</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>248</v>
@@ -8050,7 +8050,7 @@
         <v>249</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -8060,7 +8060,7 @@
         <v>250</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>251</v>

</xml_diff>